<commit_message>
Excel file for Metrics value
</commit_message>
<xml_diff>
--- a/Classes/Metrics val.xlsx
+++ b/Classes/Metrics val.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,511 +459,733 @@
           <t>CORRELATION</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>HISTOGRAM_VARIANCE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>NPCR</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>UACI</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>5.1.10.tiff</t>
+          <t>6.1.01.tiff</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.23117716342462</v>
+        <v>8.156778997588813</v>
       </c>
       <c r="C2" t="n">
-        <v>105.6394500732422</v>
+        <v>105.0476531982422</v>
       </c>
       <c r="D2" t="n">
-        <v>0.007969840369582818</v>
+        <v>0.007559322763799163</v>
       </c>
       <c r="E2" t="n">
-        <v>7.995576246553931</v>
+        <v>7.993019045411336</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.004108210209782912</v>
+        <v>0.0002945513075038</v>
+      </c>
+      <c r="G2" t="n">
+        <v>641.116124567474</v>
+      </c>
+      <c r="H2" t="n">
+        <v>99.66888427734375</v>
+      </c>
+      <c r="I2" t="n">
+        <v>33.41211655560662</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>5.1.11.tiff</t>
+          <t>Aerial.tiff</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>7.700057863821832</v>
+        <v>9.23117716342462</v>
       </c>
       <c r="C3" t="n">
-        <v>105.4205017089844</v>
+        <v>105.6394500732422</v>
       </c>
       <c r="D3" t="n">
-        <v>0.008077793673996381</v>
+        <v>0.007969840369582818</v>
       </c>
       <c r="E3" t="n">
-        <v>7.98969225199809</v>
+        <v>7.995576246553931</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.001681104114651707</v>
+        <v>-0.004108210209782912</v>
+      </c>
+      <c r="G3" t="n">
+        <v>404.7654286812764</v>
+      </c>
+      <c r="H3" t="n">
+        <v>99.56207275390625</v>
+      </c>
+      <c r="I3" t="n">
+        <v>33.62072514552696</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>5.1.12.tiff</t>
+          <t>Aerial512.tiff</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.223503761205917</v>
+        <v>8.173851793941839</v>
       </c>
       <c r="C4" t="n">
-        <v>106.2551879882812</v>
+        <v>105.5501480102539</v>
       </c>
       <c r="D4" t="n">
-        <v>0.007603752979439478</v>
+        <v>0.007912867873204462</v>
       </c>
       <c r="E4" t="n">
-        <v>7.988889079488572</v>
+        <v>7.993844373922263</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.0007939449363241238</v>
+        <v>-0.001089993672934644</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9083.962660515186</v>
+      </c>
+      <c r="H4" t="n">
+        <v>99.50180053710938</v>
+      </c>
+      <c r="I4" t="n">
+        <v>33.37418799306832</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>5.1.13.tiff</t>
+          <t>Airplane.tiff</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.075455745271743</v>
+        <v>7.700057863821832</v>
       </c>
       <c r="C5" t="n">
-        <v>105.5915222167969</v>
+        <v>105.4205017089844</v>
       </c>
       <c r="D5" t="n">
-        <v>0.007517480493097176</v>
+        <v>0.008077793673996381</v>
       </c>
       <c r="E5" t="n">
-        <v>7.731313578838155</v>
+        <v>7.98969225199809</v>
       </c>
       <c r="F5" t="n">
-        <v>0.001435207900537723</v>
+        <v>-0.001681104114651707</v>
+      </c>
+      <c r="G5" t="n">
+        <v>947.2059054209919</v>
+      </c>
+      <c r="H5" t="n">
+        <v>99.578857421875</v>
+      </c>
+      <c r="I5" t="n">
+        <v>33.65193684895834</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>5.1.14.tiff</t>
+          <t>Airplane512.tiff</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.212167315570367</v>
+        <v>8.838424511909482</v>
       </c>
       <c r="C6" t="n">
-        <v>105.563720703125</v>
+        <v>105.4510612487793</v>
       </c>
       <c r="D6" t="n">
-        <v>0.005446752314781257</v>
+        <v>0.009745887063940707</v>
       </c>
       <c r="E6" t="n">
-        <v>7.996077428765373</v>
+        <v>7.931540414743385</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.007380787365136933</v>
+        <v>-0.001784337156529359</v>
+      </c>
+      <c r="G6" t="n">
+        <v>100261.8439061899</v>
+      </c>
+      <c r="H6" t="n">
+        <v>99.57313537597656</v>
+      </c>
+      <c r="I6" t="n">
+        <v>34.3744150797526</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>5.2.08.tiff</t>
+          <t>APC512.tiff</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.593233710095811</v>
+        <v>9.772740090814745</v>
       </c>
       <c r="C7" t="n">
-        <v>105.5767555236816</v>
+        <v>105.5988731384277</v>
       </c>
       <c r="D7" t="n">
-        <v>0.009287104179924878</v>
+        <v>0.0103780066829179</v>
       </c>
       <c r="E7" t="n">
-        <v>7.996393633895227</v>
+        <v>7.986017729319951</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.001580719728598491</v>
+        <v>0.0008936406818229925</v>
+      </c>
+      <c r="G7" t="n">
+        <v>20516.7632141484</v>
+      </c>
+      <c r="H7" t="n">
+        <v>99.38392639160156</v>
+      </c>
+      <c r="I7" t="n">
+        <v>33.53911007151884</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>5.2.09.tiff</t>
+          <t>boat.512.tiff</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8.173851793941839</v>
+        <v>9.275575313728732</v>
       </c>
       <c r="C8" t="n">
-        <v>105.5501480102539</v>
+        <v>105.4716911315918</v>
       </c>
       <c r="D8" t="n">
-        <v>0.007912867873204462</v>
+        <v>0.01000876096399781</v>
       </c>
       <c r="E8" t="n">
-        <v>7.993844373922263</v>
+        <v>7.995354611728661</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.001089993672934644</v>
+        <v>0.003687502162863957</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6775.368242983468</v>
+      </c>
+      <c r="H8" t="n">
+        <v>99.50141906738281</v>
+      </c>
+      <c r="I8" t="n">
+        <v>33.28296586578968</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>5.2.10.tiff</t>
+          <t>CarAPCs1_512.tiff</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8.765354531848962</v>
+        <v>10.26772769313258</v>
       </c>
       <c r="C9" t="n">
-        <v>105.4198379516602</v>
+        <v>105.6706886291504</v>
       </c>
       <c r="D9" t="n">
-        <v>0.009261770987249804</v>
+        <v>0.01016499160758506</v>
       </c>
       <c r="E9" t="n">
-        <v>7.980706517660061</v>
+        <v>7.955389150778685</v>
       </c>
       <c r="F9" t="n">
-        <v>0.000832837947973298</v>
+        <v>-0.0003471934357054807</v>
+      </c>
+      <c r="G9" t="n">
+        <v>65789.20870434448</v>
+      </c>
+      <c r="H9" t="n">
+        <v>99.32403564453125</v>
+      </c>
+      <c r="I9" t="n">
+        <v>33.66560244092754</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>6.1.01.tiff</t>
+          <t>CarAPCs_512.tiff</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8.156778997588813</v>
+        <v>10.12962306499437</v>
       </c>
       <c r="C10" t="n">
-        <v>105.0476531982422</v>
+        <v>105.5632247924805</v>
       </c>
       <c r="D10" t="n">
-        <v>0.007559322763799163</v>
+        <v>0.01031677715744493</v>
       </c>
       <c r="E10" t="n">
-        <v>7.993019045411336</v>
+        <v>7.983693310550926</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0002945513075038</v>
+        <v>0.002046856030146311</v>
+      </c>
+      <c r="G10" t="n">
+        <v>24045.89004229143</v>
+      </c>
+      <c r="H10" t="n">
+        <v>99.39422607421875</v>
+      </c>
+      <c r="I10" t="n">
+        <v>33.43713199391085</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>7.1.01.tiff</t>
+          <t>Chemical_plant.tiff</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9.940937438829923</v>
+        <v>9.212167315570367</v>
       </c>
       <c r="C11" t="n">
-        <v>105.6881713867188</v>
+        <v>105.563720703125</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01026499710230641</v>
+        <v>0.005446752314781257</v>
       </c>
       <c r="E11" t="n">
-        <v>7.98644140774225</v>
+        <v>7.996077428765373</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00130869452956219</v>
+        <v>-0.007380787365136933</v>
+      </c>
+      <c r="G11" t="n">
+        <v>357.6086735870819</v>
+      </c>
+      <c r="H11" t="n">
+        <v>99.56817626953125</v>
+      </c>
+      <c r="I11" t="n">
+        <v>33.14146752450981</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>7.1.02.tiff</t>
+          <t>Clock.tiff</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8.838424511909482</v>
+        <v>7.223503761205917</v>
       </c>
       <c r="C12" t="n">
-        <v>105.4510612487793</v>
+        <v>106.2551879882812</v>
       </c>
       <c r="D12" t="n">
-        <v>0.009745887063940707</v>
+        <v>0.007603752979439478</v>
       </c>
       <c r="E12" t="n">
-        <v>7.931540414743385</v>
+        <v>7.988889079488572</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.001784337156529359</v>
+        <v>-0.0007939449363241238</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1028.393633217993</v>
+      </c>
+      <c r="H12" t="n">
+        <v>99.43084716796875</v>
+      </c>
+      <c r="I12" t="n">
+        <v>33.2638370289522</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>7.1.03.tiff</t>
+          <t>Couple.tiff</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>10.09596674981244</v>
+        <v>9.593233710095811</v>
       </c>
       <c r="C13" t="n">
-        <v>105.3793525695801</v>
+        <v>105.5767555236816</v>
       </c>
       <c r="D13" t="n">
-        <v>0.009606588336180808</v>
+        <v>0.009287104179924878</v>
       </c>
       <c r="E13" t="n">
-        <v>7.976850258422874</v>
+        <v>7.996393633895227</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.001493196028722689</v>
+        <v>-0.001580719728598491</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5300.115340253748</v>
+      </c>
+      <c r="H13" t="n">
+        <v>99.560546875</v>
+      </c>
+      <c r="I13" t="n">
+        <v>33.52138294893152</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>7.1.04.tiff</t>
+          <t>gray21.512.tiff</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9.772740090814745</v>
+        <v>7.581761094389405</v>
       </c>
       <c r="C14" t="n">
-        <v>105.5988731384277</v>
+        <v>105.4107704162598</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0103780066829179</v>
+        <v>0.008125846554992003</v>
       </c>
       <c r="E14" t="n">
-        <v>7.986017729319951</v>
+        <v>7.967006975055557</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0008936406818229925</v>
+        <v>0.00269277671513107</v>
+      </c>
+      <c r="G14" t="n">
+        <v>48331.43781622453</v>
+      </c>
+      <c r="H14" t="n">
+        <v>99.55024719238281</v>
+      </c>
+      <c r="I14" t="n">
+        <v>33.31559573902803</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>7.1.05.tiff</t>
+          <t>Moon_256.tiff</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9.570980281418064</v>
+        <v>10.11697339965389</v>
       </c>
       <c r="C15" t="n">
-        <v>105.5757217407227</v>
+        <v>105.7922058105469</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01053406707997141</v>
+        <v>0.01149913499084049</v>
       </c>
       <c r="E15" t="n">
-        <v>7.991691195245294</v>
+        <v>7.995315195510237</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0007599210695027543</v>
+        <v>0.002541187748652892</v>
+      </c>
+      <c r="G15" t="n">
+        <v>426.080061514802</v>
+      </c>
+      <c r="H15" t="n">
+        <v>99.462890625</v>
+      </c>
+      <c r="I15" t="n">
+        <v>33.62401625689338</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>7.1.06.tiff</t>
+          <t>Resolution_chart.tiff</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9.137623429600824</v>
+        <v>5.075455745271743</v>
       </c>
       <c r="C16" t="n">
-        <v>105.5090560913086</v>
+        <v>105.5915222167969</v>
       </c>
       <c r="D16" t="n">
-        <v>0.009540003759556928</v>
+        <v>0.007517480493097176</v>
       </c>
       <c r="E16" t="n">
-        <v>7.992894890550668</v>
+        <v>7.731313578838155</v>
       </c>
       <c r="F16" t="n">
-        <v>0.001323941815422989</v>
+        <v>0.001435207900537723</v>
+      </c>
+      <c r="G16" t="n">
+        <v>27466.42798923491</v>
+      </c>
+      <c r="H16" t="n">
+        <v>99.9542236328125</v>
+      </c>
+      <c r="I16" t="n">
+        <v>46.07293820848652</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>7.1.07.tiff</t>
+          <t>ruler.512.tiff</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>10.03672480097016</v>
+        <v>4.809952977881065</v>
       </c>
       <c r="C17" t="n">
-        <v>105.7082977294922</v>
+        <v>107.4700088500977</v>
       </c>
       <c r="D17" t="n">
-        <v>0.009367194069846192</v>
+        <v>0.03242234337353897</v>
       </c>
       <c r="E17" t="n">
-        <v>7.986213130618101</v>
+        <v>7.367217917872677</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0005680859479606264</v>
+        <v>0.04059868488305154</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1027000.308189158</v>
+      </c>
+      <c r="H17" t="n">
+        <v>100</v>
+      </c>
+      <c r="I17" t="n">
+        <v>45.09413924871706</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>7.1.08.tiff</t>
+          <t>StreamandBridge512.tiff</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>10.26772769313258</v>
+        <v>8.765354531848962</v>
       </c>
       <c r="C18" t="n">
-        <v>105.6706886291504</v>
+        <v>105.4198379516602</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01016499160758506</v>
+        <v>0.009261770987249804</v>
       </c>
       <c r="E18" t="n">
-        <v>7.955389150778685</v>
+        <v>7.980706517660061</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.0003471934357054807</v>
+        <v>0.000832837947973298</v>
+      </c>
+      <c r="G18" t="n">
+        <v>28343.48536716648</v>
+      </c>
+      <c r="H18" t="n">
+        <v>99.29237365722656</v>
+      </c>
+      <c r="I18" t="n">
+        <v>33.41863893995098</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>7.1.09.tiff</t>
+          <t>Tank1_512.tiff</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>9.77020087941524</v>
+        <v>10.03672480097016</v>
       </c>
       <c r="C19" t="n">
-        <v>105.2868003845215</v>
+        <v>105.7082977294922</v>
       </c>
       <c r="D19" t="n">
-        <v>0.009424441825384112</v>
+        <v>0.009367194069846192</v>
       </c>
       <c r="E19" t="n">
-        <v>7.989410828144559</v>
+        <v>7.986213130618101</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.001267870697635909</v>
+        <v>-0.0005680859479606264</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20191.6186082276</v>
+      </c>
+      <c r="H19" t="n">
+        <v>99.45182800292969</v>
+      </c>
+      <c r="I19" t="n">
+        <v>33.24813693177466</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>7.1.10.tiff</t>
+          <t>Tank2_512.tiff</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10.12962306499437</v>
+        <v>9.77020087941524</v>
       </c>
       <c r="C20" t="n">
-        <v>105.5632247924805</v>
+        <v>105.2868003845215</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01031677715744493</v>
+        <v>0.009424441825384112</v>
       </c>
       <c r="E20" t="n">
-        <v>7.983693310550926</v>
+        <v>7.989410828144559</v>
       </c>
       <c r="F20" t="n">
-        <v>0.002046856030146311</v>
+        <v>-0.001267870697635909</v>
+      </c>
+      <c r="G20" t="n">
+        <v>15572.62665128797</v>
+      </c>
+      <c r="H20" t="n">
+        <v>99.066162109375</v>
+      </c>
+      <c r="I20" t="n">
+        <v>33.19874782188266</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>boat.512.tiff</t>
+          <t>Tank512.tiff</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9.275575313728732</v>
+        <v>10.09596674981244</v>
       </c>
       <c r="C21" t="n">
-        <v>105.4716911315918</v>
+        <v>105.3793525695801</v>
       </c>
       <c r="D21" t="n">
-        <v>0.01000876096399781</v>
+        <v>0.009606588336180808</v>
       </c>
       <c r="E21" t="n">
-        <v>7.995354611728661</v>
+        <v>7.976850258422874</v>
       </c>
       <c r="F21" t="n">
-        <v>0.003687502162863957</v>
+        <v>-0.001493196028722689</v>
+      </c>
+      <c r="G21" t="n">
+        <v>33868.32166089965</v>
+      </c>
+      <c r="H21" t="n">
+        <v>99.03945922851562</v>
+      </c>
+      <c r="I21" t="n">
+        <v>33.43890620212929</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>gray21.512.tiff</t>
+          <t>Truck512.tiff</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>7.581761094389405</v>
+        <v>9.940937438829923</v>
       </c>
       <c r="C22" t="n">
-        <v>105.4107704162598</v>
+        <v>105.6881713867188</v>
       </c>
       <c r="D22" t="n">
-        <v>0.008125846554992003</v>
+        <v>0.01026499710230641</v>
       </c>
       <c r="E22" t="n">
-        <v>7.967006975055557</v>
+        <v>7.98644140774225</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00269277671513107</v>
+        <v>0.00130869452956219</v>
+      </c>
+      <c r="G22" t="n">
+        <v>19691.42945021146</v>
+      </c>
+      <c r="H22" t="n">
+        <v>99.43313598632812</v>
+      </c>
+      <c r="I22" t="n">
+        <v>33.45802007936964</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Moon_256.tiff</t>
+          <t>TruckAPCs1_512.tiff</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>10.11697339965389</v>
+        <v>9.137623429600824</v>
       </c>
       <c r="C23" t="n">
-        <v>105.7922058105469</v>
+        <v>105.5090560913086</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01149913499084049</v>
+        <v>0.009540003759556928</v>
       </c>
       <c r="E23" t="n">
-        <v>7.995315195510237</v>
+        <v>7.992894890550668</v>
       </c>
       <c r="F23" t="n">
-        <v>0.002541187748652892</v>
+        <v>0.001323941815422989</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10410.02100730488</v>
+      </c>
+      <c r="H23" t="n">
+        <v>99.530029296875</v>
+      </c>
+      <c r="I23" t="n">
+        <v>33.36989010081572</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>ruler.512.tiff</t>
+          <t>TruckAPCs512.tiff</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>4.809952977881065</v>
+        <v>9.570980281418064</v>
       </c>
       <c r="C24" t="n">
-        <v>107.4700088500977</v>
+        <v>105.5757217407227</v>
       </c>
       <c r="D24" t="n">
-        <v>0.03242234337353897</v>
+        <v>0.01053406707997141</v>
       </c>
       <c r="E24" t="n">
-        <v>7.367217917872677</v>
+        <v>7.991691195245294</v>
       </c>
       <c r="F24" t="n">
-        <v>0.04059868488305154</v>
+        <v>0.0007599210695027543</v>
+      </c>
+      <c r="G24" t="n">
+        <v>12183.98585159554</v>
+      </c>
+      <c r="H24" t="n">
+        <v>99.49302673339844</v>
+      </c>
+      <c r="I24" t="n">
+        <v>33.52707956351486</v>
       </c>
     </row>
   </sheetData>

</xml_diff>